<commit_message>
Actualizacion de Cronograma dia 7/05/2020
</commit_message>
<xml_diff>
--- a/Cronograma Proyecto Nomina Fase II.xlsx
+++ b/Cronograma Proyecto Nomina Fase II.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
   <si>
     <t>Modificacion de Matriz utilizando objetos</t>
   </si>
@@ -222,6 +222,27 @@
   </si>
   <si>
     <t>Graficas de usuarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base de datos utilizando Google Cloud </t>
+  </si>
+  <si>
+    <t>Aplicación de conceptos</t>
+  </si>
+  <si>
+    <t>Mejora de Diseño</t>
+  </si>
+  <si>
+    <t>Fase de Mejora Nivel III</t>
+  </si>
+  <si>
+    <t>Manual de usuario para opcion de ayuda</t>
+  </si>
+  <si>
+    <t>Promedio de Trabajo:</t>
+  </si>
+  <si>
+    <t>CRONOGRAMA DE ACTIVIDADES, PROYECTO NOMINA</t>
   </si>
 </sst>
 </file>
@@ -231,7 +252,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +274,14 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,8 +290,8 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -299,7 +328,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -405,11 +434,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -445,12 +505,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -485,7 +539,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -517,6 +570,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -538,11 +603,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -826,10 +915,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="B2:G61"/>
+  <dimension ref="B1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -843,62 +932,52 @@
     <col min="8" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="49"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="48" t="s">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="50"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="50"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="E3" s="49"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="51"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="14">
-        <v>43868</v>
-      </c>
-      <c r="E4" s="14">
-        <v>43868</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="22">
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
-        <v>2</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="D5" s="14">
         <v>43868</v>
@@ -907,18 +986,18 @@
         <v>43868</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="22">
+        <v>15</v>
+      </c>
+      <c r="G5" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>2</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="D6" s="14">
         <v>43868</v>
@@ -929,56 +1008,58 @@
       <c r="F6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
-        <v>3</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="18"/>
+        <v>2.1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="14">
+        <v>43868</v>
+      </c>
+      <c r="E7" s="14">
+        <v>43868</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="36"/>
+        <v>3</v>
+      </c>
+      <c r="C8" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="33"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="43"/>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="14">
-        <v>43871</v>
-      </c>
-      <c r="E9" s="14">
-        <v>43872</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="22">
-        <v>1</v>
-      </c>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="16"/>
     </row>
     <row r="10" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="44"/>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="14">
         <v>43871</v>
@@ -989,108 +1070,108 @@
       <c r="F10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="44"/>
-      <c r="C11" s="24" t="s">
+      <c r="B11" s="45"/>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="14">
+        <v>43871</v>
+      </c>
+      <c r="E11" s="14">
+        <v>43872</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="45"/>
+      <c r="C12" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="22"/>
-    </row>
-    <row r="12" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="44"/>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="20"/>
+    </row>
+    <row r="13" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="45"/>
+      <c r="C13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D13" s="31">
         <v>44114</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E13" s="31">
         <v>43878</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="44"/>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="34">
-        <v>44114</v>
-      </c>
-      <c r="E13" s="34">
-        <v>43878</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="22">
+      <c r="G13" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="45"/>
       <c r="C14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="34">
+        <v>36</v>
+      </c>
+      <c r="D14" s="31">
         <v>44114</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="31">
         <v>43878</v>
       </c>
       <c r="F14" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="3">
+      <c r="G14" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="46"/>
+      <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="31">
+        <v>44114</v>
+      </c>
+      <c r="E15" s="31">
+        <v>43878</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
         <v>3.2</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C16" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="21"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="46"/>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="33"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="19"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="47"/>
+      <c r="C17" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D16" s="14">
-        <v>43871</v>
-      </c>
-      <c r="E16" s="14">
-        <v>43872</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="51"/>
-      <c r="C17" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D17" s="14">
         <v>43871</v>
@@ -1101,65 +1182,65 @@
       <c r="F17" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="47"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="34">
+        <v>19</v>
+      </c>
+      <c r="D18" s="14">
         <v>43871</v>
       </c>
-      <c r="E18" s="34">
-        <v>43878</v>
+      <c r="E18" s="14">
+        <v>43872</v>
       </c>
       <c r="F18" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="3">
+      <c r="B19" s="48"/>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="31">
+        <v>43871</v>
+      </c>
+      <c r="E19" s="31">
+        <v>43878</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
         <v>3.3</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="21"/>
-    </row>
-    <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="43"/>
-      <c r="C20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="34">
-        <v>44114</v>
-      </c>
-      <c r="E20" s="14">
-        <v>43872</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="22">
-        <v>1</v>
-      </c>
+      <c r="D20" s="33"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="19"/>
     </row>
     <row r="21" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="44"/>
       <c r="C21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="14">
-        <v>43871</v>
+        <v>18</v>
+      </c>
+      <c r="D21" s="31">
+        <v>44114</v>
       </c>
       <c r="E21" s="14">
         <v>43872</v>
@@ -1167,65 +1248,65 @@
       <c r="F21" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="45"/>
       <c r="C22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="14">
         <v>43871</v>
       </c>
-      <c r="E22" s="34">
-        <v>43878</v>
+      <c r="E22" s="14">
+        <v>43872</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="3">
+      <c r="G22" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="46"/>
+      <c r="C23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="14">
+        <v>43871</v>
+      </c>
+      <c r="E23" s="31">
+        <v>43878</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
         <v>3.4</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C24" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="36"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="21"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="46"/>
-      <c r="C24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="34">
-        <v>44114</v>
-      </c>
-      <c r="E24" s="14">
-        <v>43872</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="22">
-        <v>1</v>
-      </c>
+      <c r="D24" s="33"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="19"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="47"/>
       <c r="C25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="14">
-        <v>43871</v>
+        <v>18</v>
+      </c>
+      <c r="D25" s="31">
+        <v>44114</v>
       </c>
       <c r="E25" s="14">
         <v>43872</v>
@@ -1233,450 +1314,448 @@
       <c r="F25" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G25" s="22">
+      <c r="G25" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="3">
+      <c r="B26" s="48"/>
+      <c r="C26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="14">
+        <v>43871</v>
+      </c>
+      <c r="E26" s="14">
+        <v>43872</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
         <v>4</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C27" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D27" s="31">
         <v>44117</v>
       </c>
-      <c r="E26" s="34" t="s">
+      <c r="E27" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F27" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="22"/>
+      <c r="G27" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
-      <c r="C28" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="34">
-        <v>44117</v>
-      </c>
-      <c r="E28" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="22">
-        <v>1</v>
-      </c>
+      <c r="C28" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="20"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
-      <c r="C29" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="34">
+      <c r="C29" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="31">
         <v>44117</v>
       </c>
-      <c r="E29" s="34" t="s">
-        <v>42</v>
+      <c r="E29" s="31" t="s">
+        <v>40</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="22">
+        <v>13</v>
+      </c>
+      <c r="G29" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="20"/>
+      <c r="C30" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="31">
+        <v>44117</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="10">
+      <c r="B31" s="3"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="18"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="10">
         <v>5</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C32" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="34">
+      <c r="D32" s="31">
         <v>44117</v>
       </c>
-      <c r="E31" s="34">
+      <c r="E32" s="31">
         <v>43879</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F32" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G31" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="3">
+      <c r="G32" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="3">
         <v>6</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C33" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D32" s="34">
+      <c r="D33" s="31">
         <v>44117</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E33" s="31">
         <v>43879</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="F33" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G32" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="10">
+      <c r="G33" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="10">
         <v>7</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" s="14">
+      <c r="C34" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="14">
         <v>43871</v>
       </c>
-      <c r="E33" s="34">
-        <v>43876</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="3">
-        <v>8</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="34">
-        <v>43876</v>
-      </c>
-      <c r="E34" s="34">
+      <c r="E34" s="31">
         <v>43876</v>
       </c>
       <c r="F34" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G34" s="22">
+      <c r="G34" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
-        <v>9</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="34">
+        <v>8</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="31">
         <v>43876</v>
       </c>
-      <c r="E35" s="34">
-        <v>43877</v>
+      <c r="E35" s="31">
+        <v>43876</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G35" s="22">
+        <v>15</v>
+      </c>
+      <c r="G35" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
-        <v>10</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="34">
-        <v>43878</v>
-      </c>
-      <c r="E36" s="34">
+        <v>9</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="31">
+        <v>43876</v>
+      </c>
+      <c r="E36" s="31">
         <v>43877</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G36" s="22">
+        <v>24</v>
+      </c>
+      <c r="G36" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="3">
+        <v>10</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="31">
+        <v>43878</v>
+      </c>
+      <c r="E37" s="31">
+        <v>43877</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="3">
         <v>11</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C38" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="34">
+      <c r="D38" s="31">
         <v>43876</v>
       </c>
-      <c r="E37" s="34">
+      <c r="E38" s="31">
         <v>43880</v>
       </c>
-      <c r="F37" s="15" t="s">
+      <c r="F38" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G37" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="3">
-        <v>12</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D38" s="37"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="21"/>
+      <c r="G38" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
+        <v>12</v>
+      </c>
+      <c r="C39" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="34"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="19"/>
+    </row>
+    <row r="40" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="3">
         <v>12.1</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C40" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="34">
+      <c r="D40" s="31">
         <v>43878</v>
       </c>
-      <c r="E39" s="34">
+      <c r="E40" s="31">
         <v>43880</v>
       </c>
-      <c r="F39" s="15" t="s">
+      <c r="F40" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G39" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="3">
+      <c r="G40" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
         <v>13</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C41" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="39">
+      <c r="D41" s="36">
         <v>43878</v>
       </c>
-      <c r="E40" s="34">
+      <c r="E41" s="31">
         <v>43880</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F41" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G40" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="31"/>
-      <c r="C41" s="53" t="s">
+      <c r="G41" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="29"/>
+      <c r="C42" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="27">
-        <f>B40+1</f>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="25">
+        <f>B41+1</f>
         <v>14</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="14">
+      <c r="D43" s="14">
         <v>43893</v>
-      </c>
-      <c r="E42" s="14">
-        <v>43899</v>
-      </c>
-      <c r="F42" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="G42" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="27">
-        <f>B42+1</f>
-        <v>15</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" s="14">
-        <v>43899</v>
       </c>
       <c r="E43" s="14">
         <v>43899</v>
       </c>
-      <c r="F43" s="42" t="s">
+      <c r="F43" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="G43" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="25">
+        <f>B43+1</f>
         <v>15</v>
       </c>
-      <c r="G43" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="27">
-        <f>B43+1</f>
+      <c r="C44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="14">
+        <v>43899</v>
+      </c>
+      <c r="E44" s="14">
+        <v>43899</v>
+      </c>
+      <c r="F44" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="25">
+        <f>B44+1</f>
         <v>16</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D44" s="14">
+      <c r="D45" s="14">
         <v>43900</v>
       </c>
-      <c r="E44" s="14">
+      <c r="E45" s="14">
         <v>43906</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G44" s="22">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="27">
-        <f>B44+1</f>
-        <v>17</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" s="14">
-        <v>43907</v>
-      </c>
-      <c r="E45" s="14">
-        <v>43913</v>
       </c>
       <c r="F45" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G45" s="22">
-        <v>1</v>
+      <c r="G45" s="20">
+        <v>0.75</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="27">
-        <f t="shared" ref="B46:B48" si="0">B45+1</f>
+      <c r="B46" s="25">
+        <f>B45+1</f>
+        <v>17</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="14">
+        <v>43907</v>
+      </c>
+      <c r="E46" s="14">
+        <v>43913</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="25">
+        <f t="shared" ref="B47:B49" si="0">B46+1</f>
         <v>18</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D46" s="14">
+      <c r="D47" s="14">
         <v>43913</v>
       </c>
-      <c r="E46" s="14">
+      <c r="E47" s="14">
         <v>43920</v>
       </c>
-      <c r="F46" s="15" t="s">
+      <c r="F47" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G46" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="27">
+      <c r="G47" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="25">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="14">
+      <c r="D48" s="14">
         <v>43920</v>
       </c>
-      <c r="E47" s="14">
+      <c r="E48" s="14">
         <v>43922</v>
       </c>
-      <c r="F47" s="40" t="s">
+      <c r="F48" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G47" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="27">
+      <c r="G48" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="25">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C48" s="54" t="s">
+      <c r="C49" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D48" s="40"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="28">
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="26">
         <v>20.100000000000001</v>
       </c>
-      <c r="C49" s="35" t="s">
+      <c r="C50" s="32" t="s">
         <v>53</v>
-      </c>
-      <c r="D49" s="14">
-        <v>43939</v>
-      </c>
-      <c r="E49" s="14">
-        <v>43944</v>
-      </c>
-      <c r="F49" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="G49" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="28">
-        <v>20.2</v>
-      </c>
-      <c r="C50" s="35" t="s">
-        <v>54</v>
       </c>
       <c r="D50" s="14">
         <v>43939</v>
@@ -1684,19 +1763,19 @@
       <c r="E50" s="14">
         <v>43944</v>
       </c>
-      <c r="F50" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="G50" s="22">
+      <c r="F50" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="G50" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="28">
-        <v>20.3</v>
-      </c>
-      <c r="C51" s="35" t="s">
-        <v>55</v>
+      <c r="B51" s="26">
+        <v>20.2</v>
+      </c>
+      <c r="C51" s="32" t="s">
+        <v>54</v>
       </c>
       <c r="D51" s="14">
         <v>43939</v>
@@ -1704,19 +1783,19 @@
       <c r="E51" s="14">
         <v>43944</v>
       </c>
-      <c r="F51" s="40" t="s">
+      <c r="F51" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G51" s="22">
+      <c r="G51" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="28">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="C52" s="35" t="s">
-        <v>56</v>
+      <c r="B52" s="26">
+        <v>20.3</v>
+      </c>
+      <c r="C52" s="32" t="s">
+        <v>55</v>
       </c>
       <c r="D52" s="14">
         <v>43939</v>
@@ -1724,19 +1803,19 @@
       <c r="E52" s="14">
         <v>43944</v>
       </c>
-      <c r="F52" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="G52" s="22">
+      <c r="F52" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G52" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="28">
-        <v>20.5</v>
-      </c>
-      <c r="C53" s="35" t="s">
-        <v>57</v>
+      <c r="B53" s="26">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="C53" s="32" t="s">
+        <v>56</v>
       </c>
       <c r="D53" s="14">
         <v>43939</v>
@@ -1744,19 +1823,19 @@
       <c r="E53" s="14">
         <v>43944</v>
       </c>
-      <c r="F53" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="G53" s="22">
-        <v>0.9</v>
+      <c r="F53" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="G53" s="20">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="28">
-        <v>20.6</v>
-      </c>
-      <c r="C54" s="35" t="s">
-        <v>58</v>
+      <c r="B54" s="26">
+        <v>20.5</v>
+      </c>
+      <c r="C54" s="32" t="s">
+        <v>57</v>
       </c>
       <c r="D54" s="14">
         <v>43939</v>
@@ -1764,40 +1843,39 @@
       <c r="E54" s="14">
         <v>43944</v>
       </c>
-      <c r="F54" s="40" t="s">
+      <c r="F54" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="G54" s="22">
+      <c r="G54" s="20">
         <v>0.9</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="29">
-        <v>21</v>
-      </c>
-      <c r="C55" s="35" t="s">
-        <v>65</v>
+      <c r="B55" s="26">
+        <v>20.6</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>58</v>
       </c>
       <c r="D55" s="14">
-        <v>43944</v>
+        <v>43939</v>
       </c>
       <c r="E55" s="14">
         <v>43944</v>
       </c>
-      <c r="F55" s="42" t="s">
+      <c r="F55" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="G55" s="22">
+      <c r="G55" s="20">
         <v>0.9</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="29">
-        <f>B55+1</f>
-        <v>22</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>63</v>
+      <c r="B56" s="27">
+        <v>21</v>
+      </c>
+      <c r="C56" s="32" t="s">
+        <v>65</v>
       </c>
       <c r="D56" s="14">
         <v>43944</v>
@@ -1805,115 +1883,239 @@
       <c r="E56" s="14">
         <v>43944</v>
       </c>
-      <c r="F56" s="40" t="s">
+      <c r="F56" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G56" s="20">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="27">
+        <f>B56+1</f>
+        <v>22</v>
+      </c>
+      <c r="C57" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="14">
+        <v>43944</v>
+      </c>
+      <c r="E57" s="14">
+        <v>43944</v>
+      </c>
+      <c r="F57" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="G56" s="22">
+      <c r="G57" s="20">
         <v>0.65</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="29">
-        <f>B56+1</f>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="27">
+        <f>B57+1</f>
         <v>23</v>
       </c>
-      <c r="C57" s="52" t="s">
+      <c r="C58" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="D57" s="40"/>
-      <c r="E57" s="40"/>
-      <c r="F57" s="41"/>
-      <c r="G57" s="3"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="28">
+      <c r="D58" s="53"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="38"/>
+      <c r="G58" s="3"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="26">
         <v>23.1</v>
       </c>
-      <c r="C58" s="32" t="s">
+      <c r="C59" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D58" s="14">
-        <v>43927</v>
-      </c>
-      <c r="E58" s="14">
-        <v>43931</v>
-      </c>
-      <c r="F58" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="G58" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="28">
-        <v>23.2</v>
-      </c>
-      <c r="C59" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="D59" s="14">
+      <c r="D59" s="54">
         <v>43927</v>
       </c>
       <c r="E59" s="14">
         <v>43931</v>
       </c>
-      <c r="F59" s="40" t="s">
+      <c r="F59" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="G59" s="22">
+      <c r="G59" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="28">
-        <v>23.3</v>
-      </c>
-      <c r="C60" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="D60" s="14">
+      <c r="B60" s="26">
+        <v>23.2</v>
+      </c>
+      <c r="C60" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" s="54">
         <v>43927</v>
       </c>
       <c r="E60" s="14">
         <v>43931</v>
       </c>
-      <c r="F60" s="40" t="s">
+      <c r="F60" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="G60" s="22">
+      <c r="G60" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="30">
+      <c r="B61" s="26">
+        <v>23.3</v>
+      </c>
+      <c r="C61" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D61" s="14">
+        <v>43927</v>
+      </c>
+      <c r="E61" s="14">
+        <v>43931</v>
+      </c>
+      <c r="F61" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G61" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="41">
         <v>24</v>
       </c>
-      <c r="C61" s="33" t="s">
+      <c r="C62" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="D62" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="E62" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="F61" s="40" t="s">
+      <c r="F62" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="G61" s="22">
+      <c r="G62" s="20">
         <v>0.7</v>
       </c>
     </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="57"/>
+      <c r="C63" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D63" s="58"/>
+      <c r="E63" s="58"/>
+      <c r="F63" s="58"/>
+      <c r="G63" s="59"/>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="40">
+        <v>25</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D64" s="14">
+        <v>43958</v>
+      </c>
+      <c r="E64" s="14">
+        <v>43958</v>
+      </c>
+      <c r="F64" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="G64" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="27">
+        <f>B64+1</f>
+        <v>26</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D65" s="14">
+        <v>43958</v>
+      </c>
+      <c r="E65" s="14">
+        <v>43958</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G65" s="60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="27">
+        <f t="shared" ref="B66:B67" si="1">B65+1</f>
+        <v>27</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D66" s="14">
+        <v>43958</v>
+      </c>
+      <c r="E66" s="14">
+        <v>43958</v>
+      </c>
+      <c r="F66" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G66" s="60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="28">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D67" s="14">
+        <v>43958</v>
+      </c>
+      <c r="E67" s="14">
+        <v>43958</v>
+      </c>
+      <c r="F67" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G67" s="60">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F72" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="G72" s="63">
+        <f>AVERAGE(G5:G67)</f>
+        <v>0.97199999999999986</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="B16:B18"/>
+  <mergeCells count="8">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="B17:B19"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregando Reloj, Calendario, Agenda Actividades
</commit_message>
<xml_diff>
--- a/Cronograma Proyecto Nomina Fase II.xlsx
+++ b/Cronograma Proyecto Nomina Fase II.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
   <si>
     <t>Modificacion de Matriz utilizando objetos</t>
   </si>
@@ -218,9 +218,6 @@
     <t>Verificacion de condiciones y validaciones</t>
   </si>
   <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
     <t>Graficas de usuarios</t>
   </si>
   <si>
@@ -243,6 +240,33 @@
   </si>
   <si>
     <t>CRONOGRAMA DE ACTIVIDADES, PROYECTO NOMINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultima semana </t>
+  </si>
+  <si>
+    <t>Modo vista en campos de password dentro del login</t>
+  </si>
+  <si>
+    <t>Adicion de calendario y reloj a interfaz principal</t>
+  </si>
+  <si>
+    <t>Comprobacion de validaciones y correccion de errores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adaptacion de agenda de actividades </t>
+  </si>
+  <si>
+    <t>Fecha de inicio del proyecto:</t>
+  </si>
+  <si>
+    <t>Fecha de Finalizacion esperada:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rediseño Nomina (Combobox, Iconos) </t>
+  </si>
+  <si>
+    <t>Modificacion Final de la Base de datos (Tabla Actividades)</t>
   </si>
 </sst>
 </file>
@@ -296,7 +320,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,8 +351,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -424,32 +460,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -469,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -532,9 +546,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -564,24 +575,69 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -603,36 +659,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -915,10 +943,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="B1:G72"/>
+  <dimension ref="B1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -933,24 +961,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="65" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
+      <c r="B1" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="50"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="49" t="s">
+      <c r="B3" s="68"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="69"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
@@ -1036,10 +1064,10 @@
       <c r="B8" s="3">
         <v>3</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="33"/>
+      <c r="D8" s="32"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="16"/>
@@ -1051,13 +1079,13 @@
       <c r="C9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="33"/>
+      <c r="D9" s="32"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="16"/>
     </row>
     <row r="10" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="44"/>
+      <c r="B10" s="62"/>
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1075,7 +1103,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="45"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1093,7 +1121,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="45"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="22" t="s">
         <v>20</v>
       </c>
@@ -1103,14 +1131,14 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="45"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="30">
         <v>44114</v>
       </c>
-      <c r="E13" s="31">
+      <c r="E13" s="30">
         <v>43878</v>
       </c>
       <c r="F13" s="15" t="s">
@@ -1121,14 +1149,14 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="45"/>
+      <c r="B14" s="63"/>
       <c r="C14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="30">
         <v>44114</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="30">
         <v>43878</v>
       </c>
       <c r="F14" s="15" t="s">
@@ -1139,14 +1167,14 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="46"/>
+      <c r="B15" s="64"/>
       <c r="C15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="30">
         <v>44114</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="30">
         <v>43878</v>
       </c>
       <c r="F15" s="15" t="s">
@@ -1163,13 +1191,13 @@
       <c r="C16" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="33"/>
+      <c r="D16" s="32"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="19"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
+      <c r="B17" s="65"/>
       <c r="C17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1187,7 +1215,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="52"/>
+      <c r="B18" s="70"/>
       <c r="C18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1205,14 +1233,14 @@
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="48"/>
+      <c r="B19" s="66"/>
       <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="30">
         <v>43871</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="30">
         <v>43878</v>
       </c>
       <c r="F19" s="15" t="s">
@@ -1229,17 +1257,17 @@
       <c r="C20" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="33"/>
+      <c r="D20" s="32"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="19"/>
     </row>
     <row r="21" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="44"/>
+      <c r="B21" s="62"/>
       <c r="C21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="30">
         <v>44114</v>
       </c>
       <c r="E21" s="14">
@@ -1253,7 +1281,7 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="45"/>
+      <c r="B22" s="63"/>
       <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1271,14 +1299,14 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="46"/>
+      <c r="B23" s="64"/>
       <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="14">
         <v>43871</v>
       </c>
-      <c r="E23" s="31">
+      <c r="E23" s="30">
         <v>43878</v>
       </c>
       <c r="F23" s="15" t="s">
@@ -1295,17 +1323,17 @@
       <c r="C24" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="33"/>
+      <c r="D24" s="32"/>
       <c r="E24" s="12"/>
       <c r="F24" s="17"/>
       <c r="G24" s="19"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
+      <c r="B25" s="65"/>
       <c r="C25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="31">
+      <c r="D25" s="30">
         <v>44114</v>
       </c>
       <c r="E25" s="14">
@@ -1319,7 +1347,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="48"/>
+      <c r="B26" s="66"/>
       <c r="C26" s="1" t="s">
         <v>19</v>
       </c>
@@ -1343,10 +1371,10 @@
       <c r="C27" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="31">
+      <c r="D27" s="30">
         <v>44117</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="30" t="s">
         <v>33</v>
       </c>
       <c r="F27" s="15" t="s">
@@ -1361,8 +1389,8 @@
       <c r="C28" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
       <c r="F28" s="15"/>
       <c r="G28" s="20"/>
     </row>
@@ -1371,10 +1399,10 @@
       <c r="C29" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="31">
+      <c r="D29" s="30">
         <v>44117</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="30" t="s">
         <v>40</v>
       </c>
       <c r="F29" s="15" t="s">
@@ -1389,10 +1417,10 @@
       <c r="C30" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="31">
+      <c r="D30" s="30">
         <v>44117</v>
       </c>
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="30" t="s">
         <v>42</v>
       </c>
       <c r="F30" s="15" t="s">
@@ -1404,8 +1432,8 @@
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
       <c r="F31" s="15"/>
       <c r="G31" s="18"/>
     </row>
@@ -1416,10 +1444,10 @@
       <c r="C32" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="31">
+      <c r="D32" s="30">
         <v>44117</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="30">
         <v>43879</v>
       </c>
       <c r="F32" s="15" t="s">
@@ -1436,10 +1464,10 @@
       <c r="C33" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D33" s="31">
+      <c r="D33" s="30">
         <v>44117</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="30">
         <v>43879</v>
       </c>
       <c r="F33" s="15" t="s">
@@ -1459,7 +1487,7 @@
       <c r="D34" s="14">
         <v>43871</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="30">
         <v>43876</v>
       </c>
       <c r="F34" s="15" t="s">
@@ -1476,10 +1504,10 @@
       <c r="C35" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="31">
+      <c r="D35" s="30">
         <v>43876</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="30">
         <v>43876</v>
       </c>
       <c r="F35" s="15" t="s">
@@ -1496,10 +1524,10 @@
       <c r="C36" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="31">
+      <c r="D36" s="30">
         <v>43876</v>
       </c>
-      <c r="E36" s="31">
+      <c r="E36" s="30">
         <v>43877</v>
       </c>
       <c r="F36" s="15" t="s">
@@ -1516,10 +1544,10 @@
       <c r="C37" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="31">
+      <c r="D37" s="30">
         <v>43878</v>
       </c>
-      <c r="E37" s="31">
+      <c r="E37" s="30">
         <v>43877</v>
       </c>
       <c r="F37" s="15" t="s">
@@ -1536,10 +1564,10 @@
       <c r="C38" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D38" s="31">
+      <c r="D38" s="30">
         <v>43876</v>
       </c>
-      <c r="E38" s="31">
+      <c r="E38" s="30">
         <v>43880</v>
       </c>
       <c r="F38" s="15" t="s">
@@ -1553,11 +1581,11 @@
       <c r="B39" s="3">
         <v>12</v>
       </c>
-      <c r="C39" s="61" t="s">
+      <c r="C39" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="34"/>
-      <c r="E39" s="35"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="34"/>
       <c r="F39" s="12"/>
       <c r="G39" s="19"/>
     </row>
@@ -1568,10 +1596,10 @@
       <c r="C40" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D40" s="31">
+      <c r="D40" s="30">
         <v>43878</v>
       </c>
-      <c r="E40" s="31">
+      <c r="E40" s="30">
         <v>43880</v>
       </c>
       <c r="F40" s="15" t="s">
@@ -1588,10 +1616,10 @@
       <c r="C41" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="36">
+      <c r="D41" s="35">
         <v>43878</v>
       </c>
-      <c r="E41" s="31">
+      <c r="E41" s="30">
         <v>43880</v>
       </c>
       <c r="F41" s="15" t="s">
@@ -1602,8 +1630,8 @@
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="29"/>
-      <c r="C42" s="42" t="s">
+      <c r="B42" s="28"/>
+      <c r="C42" s="39" t="s">
         <v>43</v>
       </c>
       <c r="D42" s="13"/>
@@ -1625,7 +1653,7 @@
       <c r="E43" s="14">
         <v>43899</v>
       </c>
-      <c r="F43" s="37" t="s">
+      <c r="F43" s="36" t="s">
         <v>62</v>
       </c>
       <c r="G43" s="20">
@@ -1646,7 +1674,7 @@
       <c r="E44" s="14">
         <v>43899</v>
       </c>
-      <c r="F44" s="39" t="s">
+      <c r="F44" s="38" t="s">
         <v>15</v>
       </c>
       <c r="G44" s="20">
@@ -1730,7 +1758,7 @@
       <c r="E48" s="14">
         <v>43922</v>
       </c>
-      <c r="F48" s="37" t="s">
+      <c r="F48" s="36" t="s">
         <v>24</v>
       </c>
       <c r="G48" s="20">
@@ -1742,19 +1770,19 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C49" s="43" t="s">
+      <c r="C49" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="D49" s="37"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="38"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="37"/>
       <c r="G49" s="3"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="26">
         <v>20.100000000000001</v>
       </c>
-      <c r="C50" s="32" t="s">
+      <c r="C50" s="31" t="s">
         <v>53</v>
       </c>
       <c r="D50" s="14">
@@ -1763,7 +1791,7 @@
       <c r="E50" s="14">
         <v>43944</v>
       </c>
-      <c r="F50" s="37" t="s">
+      <c r="F50" s="36" t="s">
         <v>62</v>
       </c>
       <c r="G50" s="20">
@@ -1774,7 +1802,7 @@
       <c r="B51" s="26">
         <v>20.2</v>
       </c>
-      <c r="C51" s="32" t="s">
+      <c r="C51" s="31" t="s">
         <v>54</v>
       </c>
       <c r="D51" s="14">
@@ -1783,7 +1811,7 @@
       <c r="E51" s="14">
         <v>43944</v>
       </c>
-      <c r="F51" s="37" t="s">
+      <c r="F51" s="36" t="s">
         <v>24</v>
       </c>
       <c r="G51" s="20">
@@ -1794,7 +1822,7 @@
       <c r="B52" s="26">
         <v>20.3</v>
       </c>
-      <c r="C52" s="32" t="s">
+      <c r="C52" s="31" t="s">
         <v>55</v>
       </c>
       <c r="D52" s="14">
@@ -1803,7 +1831,7 @@
       <c r="E52" s="14">
         <v>43944</v>
       </c>
-      <c r="F52" s="37" t="s">
+      <c r="F52" s="36" t="s">
         <v>24</v>
       </c>
       <c r="G52" s="20">
@@ -1814,7 +1842,7 @@
       <c r="B53" s="26">
         <v>20.399999999999999</v>
       </c>
-      <c r="C53" s="32" t="s">
+      <c r="C53" s="31" t="s">
         <v>56</v>
       </c>
       <c r="D53" s="14">
@@ -1823,7 +1851,7 @@
       <c r="E53" s="14">
         <v>43944</v>
       </c>
-      <c r="F53" s="37" t="s">
+      <c r="F53" s="36" t="s">
         <v>23</v>
       </c>
       <c r="G53" s="20">
@@ -1834,7 +1862,7 @@
       <c r="B54" s="26">
         <v>20.5</v>
       </c>
-      <c r="C54" s="32" t="s">
+      <c r="C54" s="31" t="s">
         <v>57</v>
       </c>
       <c r="D54" s="14">
@@ -1843,7 +1871,7 @@
       <c r="E54" s="14">
         <v>43944</v>
       </c>
-      <c r="F54" s="37" t="s">
+      <c r="F54" s="36" t="s">
         <v>22</v>
       </c>
       <c r="G54" s="20">
@@ -1854,7 +1882,7 @@
       <c r="B55" s="26">
         <v>20.6</v>
       </c>
-      <c r="C55" s="32" t="s">
+      <c r="C55" s="31" t="s">
         <v>58</v>
       </c>
       <c r="D55" s="14">
@@ -1863,7 +1891,7 @@
       <c r="E55" s="14">
         <v>43944</v>
       </c>
-      <c r="F55" s="37" t="s">
+      <c r="F55" s="36" t="s">
         <v>22</v>
       </c>
       <c r="G55" s="20">
@@ -1874,8 +1902,8 @@
       <c r="B56" s="27">
         <v>21</v>
       </c>
-      <c r="C56" s="32" t="s">
-        <v>65</v>
+      <c r="C56" s="31" t="s">
+        <v>64</v>
       </c>
       <c r="D56" s="14">
         <v>43944</v>
@@ -1883,7 +1911,7 @@
       <c r="E56" s="14">
         <v>43944</v>
       </c>
-      <c r="F56" s="39" t="s">
+      <c r="F56" s="38" t="s">
         <v>22</v>
       </c>
       <c r="G56" s="20">
@@ -1895,7 +1923,7 @@
         <f>B56+1</f>
         <v>22</v>
       </c>
-      <c r="C57" s="55" t="s">
+      <c r="C57" s="44" t="s">
         <v>63</v>
       </c>
       <c r="D57" s="14">
@@ -1904,7 +1932,7 @@
       <c r="E57" s="14">
         <v>43944</v>
       </c>
-      <c r="F57" s="37" t="s">
+      <c r="F57" s="36" t="s">
         <v>15</v>
       </c>
       <c r="G57" s="20">
@@ -1916,28 +1944,28 @@
         <f>B57+1</f>
         <v>23</v>
       </c>
-      <c r="C58" s="56" t="s">
+      <c r="C58" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="D58" s="53"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="38"/>
+      <c r="D58" s="42"/>
+      <c r="E58" s="36"/>
+      <c r="F58" s="37"/>
       <c r="G58" s="3"/>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="26">
         <v>23.1</v>
       </c>
-      <c r="C59" s="30" t="s">
+      <c r="C59" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="D59" s="54">
+      <c r="D59" s="43">
         <v>43927</v>
       </c>
       <c r="E59" s="14">
         <v>43931</v>
       </c>
-      <c r="F59" s="37" t="s">
+      <c r="F59" s="36" t="s">
         <v>15</v>
       </c>
       <c r="G59" s="20">
@@ -1948,16 +1976,16 @@
       <c r="B60" s="26">
         <v>23.2</v>
       </c>
-      <c r="C60" s="30" t="s">
+      <c r="C60" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="D60" s="54">
+      <c r="D60" s="43">
         <v>43927</v>
       </c>
       <c r="E60" s="14">
         <v>43931</v>
       </c>
-      <c r="F60" s="37" t="s">
+      <c r="F60" s="36" t="s">
         <v>15</v>
       </c>
       <c r="G60" s="20">
@@ -1968,7 +1996,7 @@
       <c r="B61" s="26">
         <v>23.3</v>
       </c>
-      <c r="C61" s="30" t="s">
+      <c r="C61" s="29" t="s">
         <v>61</v>
       </c>
       <c r="D61" s="14">
@@ -1977,7 +2005,7 @@
       <c r="E61" s="14">
         <v>43931</v>
       </c>
-      <c r="F61" s="37" t="s">
+      <c r="F61" s="36" t="s">
         <v>15</v>
       </c>
       <c r="G61" s="20">
@@ -1985,41 +2013,42 @@
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="41">
-        <v>24</v>
-      </c>
-      <c r="C62" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="D62" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="F62" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="G62" s="20">
-        <v>0.7</v>
-      </c>
+      <c r="B62" s="41"/>
+      <c r="C62" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D62" s="46"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="47"/>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="57"/>
-      <c r="C63" s="42" t="s">
+      <c r="B63" s="41">
+        <v>25</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D63" s="58"/>
-      <c r="E63" s="58"/>
-      <c r="F63" s="58"/>
-      <c r="G63" s="59"/>
+      <c r="D63" s="14">
+        <v>43958</v>
+      </c>
+      <c r="E63" s="14">
+        <v>43958</v>
+      </c>
+      <c r="F63" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="G63" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="40">
-        <v>25</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>70</v>
+      <c r="B64" s="27">
+        <f>B63+1</f>
+        <v>26</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="D64" s="14">
         <v>43958</v>
@@ -2027,17 +2056,17 @@
       <c r="E64" s="14">
         <v>43958</v>
       </c>
-      <c r="F64" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="G64" s="20">
+      <c r="F64" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G64" s="48">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" s="27">
-        <f>B64+1</f>
-        <v>26</v>
+        <f t="shared" ref="B65:B66" si="1">B64+1</f>
+        <v>27</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>66</v>
@@ -2049,16 +2078,16 @@
         <v>43958</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G65" s="60">
+        <v>23</v>
+      </c>
+      <c r="G65" s="48">
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="27">
-        <f t="shared" ref="B66:B67" si="1">B65+1</f>
-        <v>27</v>
+        <f t="shared" si="1"/>
+        <v>28</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>67</v>
@@ -2072,38 +2101,192 @@
       <c r="F66" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G66" s="60">
-        <v>1</v>
+      <c r="G66" s="48">
+        <v>0.8</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B67" s="28">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D67" s="14">
-        <v>43958</v>
-      </c>
-      <c r="E67" s="14">
-        <v>43958</v>
-      </c>
-      <c r="F67" s="15" t="s">
+      <c r="B67" s="29"/>
+      <c r="C67" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="G67" s="47"/>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="54">
+        <v>29</v>
+      </c>
+      <c r="C68" s="71" t="s">
+        <v>79</v>
+      </c>
+      <c r="D68" s="30">
+        <v>43966</v>
+      </c>
+      <c r="E68" s="30">
+        <v>43968</v>
+      </c>
+      <c r="F68" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="54">
+        <f>B68+1</f>
+        <v>30</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D69" s="56">
+        <v>43976</v>
+      </c>
+      <c r="E69" s="56">
+        <v>43976</v>
+      </c>
+      <c r="F69" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="G69" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="54">
+        <f t="shared" ref="B70:B74" si="2">B69+1</f>
+        <v>31</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D70" s="56">
+        <v>43886</v>
+      </c>
+      <c r="E70" s="56">
+        <v>43886</v>
+      </c>
+      <c r="F70" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="G70" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="54">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D71" s="56">
+        <v>43977</v>
+      </c>
+      <c r="E71" s="56">
+        <v>43977</v>
+      </c>
+      <c r="F71" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G67" s="60">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="F72" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="G72" s="63">
-        <f>AVERAGE(G5:G67)</f>
-        <v>0.97199999999999986</v>
+      <c r="G71" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="54">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D72" s="56">
+        <v>43976</v>
+      </c>
+      <c r="E72" s="56">
+        <v>43977</v>
+      </c>
+      <c r="F72" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="G72" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="54">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D73" s="56">
+        <v>43977</v>
+      </c>
+      <c r="E73" s="56">
+        <v>43978</v>
+      </c>
+      <c r="F73" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G73" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="54">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D74" s="58">
+        <v>43974</v>
+      </c>
+      <c r="E74" s="58">
+        <v>43979</v>
+      </c>
+      <c r="F74" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="G74" s="20">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="52"/>
+      <c r="E75" s="57"/>
+    </row>
+    <row r="76" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F76" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="G76" s="51">
+        <f>AVERAGE(G5:G74)</f>
+        <v>0.93928571428571417</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F78" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G78" s="60">
+        <f>D5</f>
+        <v>43868</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F79" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G79" s="60">
+        <f>E74</f>
+        <v>43979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>